<commit_message>
fixed no data bug in populate_db.js
</commit_message>
<xml_diff>
--- a/src/data/flash-dsa-data.xlsx
+++ b/src/data/flash-dsa-data.xlsx
@@ -8238,8 +8238,8 @@
   </sheetPr>
   <dimension ref="A1:I418"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E224" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I232" activeCellId="0" sqref="I232"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>